<commit_message>
avance en limpieza de nombres de candidatos
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_final1v2023.xlsx
+++ b/tesis_doctorado/datav2023/base_final1v2023.xlsx
@@ -683,7 +683,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Leonel Brizola;Luis Inácio Lula da Silva;Mário Covas;Paulo Maluf;Aureliano Chaves;Afif Domingos;Roberto Freire;Ronaldo Caiado;Affonso Camargo</t>
+          <t>Leonel Brizola;Luiz Inácio Lula da Silva;Mário Covas;Paulo Maluf;Aureliano Chaves;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Affonso Camargo</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luis Inacio Lula da Silva;Mario Covas</t>
+          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luiz Inacio Lula da Silva;Mario Covas</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luis Inacio Lula da Silva;Mario Covas</t>
+          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luiz Inacio Lula da Silva;Mario Covas</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>primero: Leonel Brizola;Paulo Maluf;Aureliano Chaves;Guillerme Afif Domingos;Roberto Freire;segundo: Mario Covas;Luis Inácio Lula da Silva;Ulysses Guimaraes;Ronaldo Caiado;Alfonso Camargo</t>
+          <t>primero: Leonel Brizola;Paulo Maluf;Aureliano Chaves;Guilherme Afif Domingos;Roberto Freire;segundo: Mario Covas;Luiz Inácio Lula da Silva;Ulysses Guimaraes;Ronaldo Caiado;Affonso Camargo</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luis Inacio Lula da Silva;Mario Covas</t>
+          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luiz Inacio Lula da Silva;Mario Covas</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luis Inacio Lula da Silva;Mario Covas;Ulysses Guimaraes;Affonso Camargo;Aureliano Chaves</t>
+          <t>Leonel Brizola;Paulo Maluf;Guilherme Afif Domingos;Roberto Freire;Ronaldo Caiado;Luiz Inacio Lula da Silva;Mario Covas;Ulysses Guimaraes;Affonso Camargo;Aureliano Chaves</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Fernando Collor de Mello;Luis Inácio Lula da Silva</t>
+          <t>Fernando Collor de Mello;Luiz Inácio Lula da Silva</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Fernando Collor de Mello;Luis Inácio Lula da Silva</t>
+          <t>Fernando Collor de Mello;Luiz Inácio Lula da Silva</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Esperidião Amin;Leonel Brizola;Enéas Ferreira Carneiro;Hernani Goulart Fortuna;Luis Inacio Lula da Silva</t>
+          <t>Esperidião Amin;Leonel Brizola;Enéas Ferreira Carneiro;Hernani Goulart Fortuna;Luiz Inacio Lula da Silva</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -5059,7 +5059,7 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Marina Silva;José Serra;Dilma Rouseff;Plinio Sampaio</t>
+          <t>Marina Silva;José Serra;Dilma Rousseff;Plinio Sampaio</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Marina Silva;José Serra;Dilma Rouseff</t>
+          <t>Marina Silva;José Serra;Dilma Rousseff</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -5487,7 +5487,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>Dilma Rouseff</t>
+          <t>Dilma Rousseff</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>Dilma Rouseff</t>
+          <t>Dilma Rousseff</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -6117,7 +6117,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>Dilma Rouseff</t>
+          <t>Dilma Rousseff</t>
         </is>
       </c>
       <c r="S29">
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff;Plinio Sampaio;Marina Silva</t>
+          <t>José Serra;Dilma Rousseff;Plinio Sampaio;Marina Silva</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff;Plinio Sampaio;Marina Silva</t>
+          <t>José Serra;Dilma Rousseff;Plinio Sampaio;Marina Silva</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
@@ -6934,7 +6934,7 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff</t>
+          <t>José Serra;Dilma Rousseff</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
@@ -7140,7 +7140,7 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff</t>
+          <t>José Serra;Dilma Rousseff</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff</t>
+          <t>José Serra;Dilma Rousseff</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
@@ -7546,7 +7546,7 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>José Serra;Dilma Rouseff</t>
+          <t>José Serra;Dilma Rousseff</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
@@ -12745,7 +12745,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Michelle Bachelet;Tomás Hirsch;Joaquín Lavín;Sebastián Piñera</t>
+          <t>Michelle Bachelet Jeria;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastián Piñera</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
@@ -13719,7 +13719,7 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Michelle Bachelet;Tomás Hirsch;Joaquín Lavín;Sebastián Piñera</t>
+          <t>Michelle Bachelet Jeria;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastián Piñera</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
@@ -15522,7 +15522,7 @@
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Franco Parisi Fernández;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
+          <t>Franco Parisi;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
         </is>
       </c>
       <c r="Q75" t="inlineStr">
@@ -15741,7 +15741,7 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Michelle Bachelet Jeria;Franco Parisi Fernández;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
+          <t>Michelle Bachelet Jeria;Franco Parisi;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
@@ -15934,7 +15934,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>el primero: Constanza Santa María;Claudio Elórtegui;Soledad Onetto; el segundo: Beatriz Sánchez;Mauricio Bustamante;Iván Núñez</t>
+          <t>el primero: Constanza Santa María;Claudio Elórtegui;Soledad Onetto; el segundo: Beatriz Sánchez Muñoz;Mauricio Bustamante;Iván Núñez</t>
         </is>
       </c>
       <c r="O77">
@@ -15942,7 +15942,7 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Michelle Bachelet Jeria;Franco Parisi Fernández;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
+          <t>Michelle Bachelet Jeria;Franco Parisi;Marcel Claude Reyes;Ricardo Israel Zipper;Marco Enríquez-Ominami Gumucio;Roxana Miranda Meneses;Evelyn Matthei Fornet;Alfredo Sfeir Younis;Tomás Jocelyn-Holt Letelier</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
@@ -16346,7 +16346,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Beatriz Sánchez;Gabriela Núñez;Mauricio Bustamante;Soledad Onetto;Iván Núñez;Ramón Ulloa</t>
+          <t>Beatriz Sánchez Muñoz;Gabriela Núñez;Mauricio Bustamante;Soledad Onetto;Iván Núñez;Ramón Ulloa</t>
         </is>
       </c>
       <c r="O79">
@@ -16548,7 +16548,7 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Michelle Bachelet Jeria;Franco Parisi Fernández;Evelyn Matthei Fornet;Marco Enríquez-Ominami Gumucio</t>
+          <t>Michelle Bachelet Jeria;Franco Parisi;Evelyn Matthei Fornet;Marco Enríquez-Ominami Gumucio</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
@@ -16706,7 +16706,7 @@
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Sebastián Piñera;Beatriz Sánchez;José Antonio Kast; Alejandro Guillier;Carolina Goic</t>
+          <t>Sebastián Piñera Echenique;Beatriz Sánchez Muñoz;José Antonio Kast;Alejandro Guillier;Carolina Goic</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
@@ -16880,7 +16880,7 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Marco Enríquez-Ominami Gumucio;Beatriz Sánchez;José Antonio Kast;Carolina Goic;Alejandro Guillier Álvarez;Eduardo Artés Brichetti;Alejandro Navarro Brain</t>
+          <t>Marco Enríquez-Ominami Gumucio;Beatriz Sánchez Muñoz;José Antonio Kast;Carolina Goic;Alejandro Guillier;Eduardo Artés;Alejandro Navarro Brain</t>
         </is>
       </c>
       <c r="Q82" t="inlineStr">
@@ -17102,7 +17102,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>Sebastián Piñera;José Antonio Kast;Carolina Goic;Alejandro Guillier Álvarez;Eduardo Artés Brichetti;Alejandro Navarro Brain</t>
+          <t>Sebastián Piñera Echenique;José Antonio Kast;Carolina Goic;Alejandro Guillier;Eduardo Artés;Alejandro Navarro Brain</t>
         </is>
       </c>
       <c r="S83">
@@ -17301,7 +17301,7 @@
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Carolina Goic Boroevic;José Antonio Kast Rist;Sebastián Piñera Echenique;Alejandro Guillier Álvarez;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés Brichetti;Alejandro Navarro Brain</t>
+          <t>Carolina Goic;José Antonio Kast;Sebastián Piñera Echenique;Alejandro Guillier;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés;Alejandro Navarro Brain</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
@@ -17518,7 +17518,7 @@
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Carolina Goic Boroevic;José Antonio Kast Rist;Sebastián Piñera Echenique;Alejandro Guillier Álvarez;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés Brichetti;Alejandro Navarro Brain</t>
+          <t>Carolina Goic;José Antonio Kast;Sebastián Piñera Echenique;Alejandro Guillier;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés;Alejandro Navarro Brain</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
@@ -17717,7 +17717,7 @@
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Carolina Goic Boroevic;José Antonio Kast Rist;Sebastián Piñera Echenique;Alejandro Guillier Álvarez;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés Brichetti;Alejandro Navarro Brain</t>
+          <t>Carolina Goic;José Antonio Kast;Sebastián Piñera Echenique;Alejandro Guillier;Beatriz Sánchez Muñoz;Marco Enríquez-Ominami Gumucio;Eduardo Artés;Alejandro Navarro Brain</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
@@ -17924,7 +17924,7 @@
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Sebastián Piñera Echenique;Alejandro Guillier Álvarez</t>
+          <t>Sebastián Piñera Echenique;Alejandro Guillier</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
@@ -18125,7 +18125,7 @@
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Sebastián Piñera Echenique;Alejandro Guillier Álvarez</t>
+          <t>Sebastián Piñera Echenique;Alejandro Guillier</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
@@ -18340,7 +18340,7 @@
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>MEO;Franco Parisi</t>
+          <t>Marco Enríquez-Ominami Gumucio;Franco Parisi</t>
         </is>
       </c>
       <c r="R89" t="inlineStr">
@@ -18537,7 +18537,7 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>MEO;Franco Parisi;Eduardo Artés;Gabriel Boric</t>
+          <t>Marco Enríquez-Ominami Gumucio;Franco Parisi;Eduardo Artés;Gabriel Boric</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
@@ -18670,7 +18670,7 @@
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>MEO;Eduardo Artés;José Antonio Kast;Sebastián Sichel;Gabriel Boric;Yasna Provoste</t>
+          <t>Marco Enríquez-Ominami Gumucio;Eduardo Artés;José Antonio Kast;Sebastián Sichel;Gabriel Boric;Yasna Provoste</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
@@ -18890,7 +18890,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>MEO;Eduardo Artés;José Antonio Kast;Sebastián Sichel;Gabriel Boric;Yasna Provoste</t>
+          <t>Marco Enríquez-Ominami Gumucio;Eduardo Artés;José Antonio Kast;Sebastián Sichel;Gabriel Boric;Yasna Provoste</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
@@ -19105,7 +19105,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>Gabriel Boric;MEO;Yasna Provoste;Sebastián Sichel;Franco Parisi</t>
+          <t>Gabriel Boric;Marco Enríquez-Ominami Gumucio;Yasna Provoste;Sebastián Sichel;Franco Parisi</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -19325,7 +19325,7 @@
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>Gabriel Boric;Yasna Provoste;Sebastián Sichel;Eduardo Artés;MEO</t>
+          <t>Gabriel Boric;Yasna Provoste;Sebastián Sichel;Eduardo Artés;Marco Enríquez-Ominami Gumucio</t>
         </is>
       </c>
       <c r="Q94" t="inlineStr">
@@ -19540,7 +19540,7 @@
       </c>
       <c r="P95" t="inlineStr">
         <is>
-          <t>Yasna Provoste;Sebastián Sichel;Eduardo Artés;MEO</t>
+          <t>Yasna Provoste;Sebastián Sichel;Eduardo Artés;Marco Enríquez-Ominami Gumucio</t>
         </is>
       </c>
       <c r="Q95" t="inlineStr">
@@ -19765,7 +19765,7 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Yasna Provoste;MEO;Gabriel Boric;José Antonio Kast;Sebastián Sichel</t>
+          <t>Yasna Provoste;Marco Enríquez-Ominami Gumucio;Gabriel Boric;José Antonio Kast;Sebastián Sichel</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr">
@@ -19975,7 +19975,7 @@
       </c>
       <c r="P97" t="inlineStr">
         <is>
-          <t>Yasna Provoste;MEO;Gabriel Boric;José Antonio Kast;Sebastián Sichel;Eduardo Artés</t>
+          <t>Yasna Provoste;Marco Enríquez-Ominami Gumucio;Gabriel Boric;José Antonio Kast;Sebastián Sichel;Eduardo Artés</t>
         </is>
       </c>
       <c r="Q97" t="inlineStr">
@@ -22027,7 +22027,7 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>Alberto Fujimori Fujimori;Mario Vargas Llosa</t>
+          <t>Alberto Fujimori;Mario Vargas Llosa</t>
         </is>
       </c>
       <c r="Q107" t="inlineStr">
@@ -22632,7 +22632,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>Keiko Fujimori Higuchi;Óscar Luis Castañeda Lossio;Pedro Pablo Kuczynski Godard;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Edith Reymer Rodríguez;Humberto Pinazo Bella;Rafael Luis Belaúnde Aubry;José Manuel Rodríguez Cuadros;Ricardo Manuel Germán Noriega Salaverry;José Antonio Ñique de la Puente</t>
+          <t>Keiko Fujimori Higuchi;Óscar Luis Castañeda Lossio;Pedro Pablo Kuczynski;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Edith Reymer Rodríguez;Humberto Pinazo Bella;Rafael Belaúnde Aubry;José Manuel Rodríguez Cuadros;Ricardo Noriega Salaverry;José Antonio Ñique de la Puente</t>
         </is>
       </c>
       <c r="Q110" t="inlineStr">
@@ -22831,7 +22831,7 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Ollanta Moisés Humala Tasso;Ricardo Noriega Salaverry;Juliana Reymer Rodríguez;Manuel Rodríguez Cuadros;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;José Ñique de la Puente;Pedro Pablo Kuczynski;Humberto Punazo Bella;Rafael Belaúnde Aubry;Luis Castañeda Lossio</t>
+          <t>Ollanta Moisés Humala Tasso;Ricardo Noriega Salaverry;Juliana Reymer Rodríguez;Manuel Rodríguez Cuadros;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;José Ñique de la Puente;Pedro Pablo Kuczynski;Humberto Pinazo Bella;Rafael Belaúnde Aubry;Luis Castañeda Lossio</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
@@ -23447,12 +23447,12 @@
       </c>
       <c r="P114" t="inlineStr">
         <is>
-          <t>primero: Ántero Flores-Aráoz;Hernando Guerra García;Francisco Diez Canseco;Yehude Simon;Fernando Olivera; segundo: Julio Guzmán; Verónika Mendoza;Vladimir Cerrón;Gregorio Santos</t>
+          <t>primero: Ántero Flores-Aráoz;Hernando Guerra García;Francisco Diez Canseco;Yehude Simon;Fernando Olivera; segundo: Julio Guzmán; Verónika Mendoza;Vladimir Cerrón;Gregorio Santos Guerrero</t>
         </is>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>ausentes a la primera: César Acuña;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;Miguel Hilario;ausentes a la segunda: Daniel Urresti Elera;Alan García;Pedro Pablo Kuczynski;Renzo Reggiardo;Alfredo Barnechea</t>
+          <t>ausentes a la primera: César Acuña;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;Miguel Hilario;ausentes a la segunda: Daniel Urresti Elera;Alan García Pérez;Pedro Pablo Kuczynski;Renzo Reggiardo;Alfredo Barnechea</t>
         </is>
       </c>
       <c r="R114" t="inlineStr">
@@ -24686,7 +24686,7 @@
       </c>
       <c r="P120" t="inlineStr">
         <is>
-          <t>primero: César Acuña;Marco Arana;Keiko Fujimori;Verónika Mendoza;Alberto Beingolea;George Forsyth; segundo: Hernando de Soto;Andrés Alcántara;Ollanta Moisés Humala Taso;José Castillo;Daniel Urresti;José Vega;tercero: Yonhy Lescano;Julio Guzmán;Rafael Santos;Ciro Gálvez;Rafael López Aliaga;Daniel Salaverry</t>
+          <t>primero: César Acuña;Marco Arana;Keiko Fujimori Higuchi;Verónika Mendoza;Alberto Beingolea;George Forsyth; segundo: Hernando de Soto;Andrés Alcántara;Ollanta Moisés Humala Tasso;José Castillo;Daniel Urresti;José Vega;tercero: Yonhy Lescano;Julio Guzmán;Rafael Santos;Ciro Gálvez;Rafael López Aliaga;Daniel Salaverry</t>
         </is>
       </c>
       <c r="Q120" t="inlineStr">
@@ -27594,7 +27594,7 @@
       </c>
       <c r="P135" t="inlineStr">
         <is>
-          <t>Sixto Durán Ballén;Jaime Roldós Aguilera</t>
+          <t>Sixto Durán Ballén;Jaime Roldós</t>
         </is>
       </c>
       <c r="Q135" t="inlineStr">
@@ -27962,12 +27962,9 @@
           <t>Cámara de Industriales de Pichincha</t>
         </is>
       </c>
-      <c r="O137">
-        <v>1</v>
-      </c>
       <c r="P137" t="inlineStr">
         <is>
-          <t>No invitado Abdalá</t>
+          <t>sin datos</t>
         </is>
       </c>
       <c r="Q137" t="inlineStr">
@@ -28026,9 +28023,6 @@
       <c r="AI137">
         <v>0</v>
       </c>
-      <c r="AJ137">
-        <v>1</v>
-      </c>
       <c r="AK137" t="inlineStr">
         <is>
           <t>NA</t>
@@ -28104,9 +28098,6 @@
       </c>
       <c r="AZ137">
         <v>12</v>
-      </c>
-      <c r="BA137">
-        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="138">
@@ -28135,12 +28126,9 @@
           <t>Cámara de la Construcción de Quito</t>
         </is>
       </c>
-      <c r="O138">
-        <v>1</v>
-      </c>
       <c r="P138" t="inlineStr">
         <is>
-          <t>No invitado Abdalá</t>
+          <t>sin datos</t>
         </is>
       </c>
       <c r="Q138" t="inlineStr">
@@ -28199,9 +28187,6 @@
       <c r="AI138">
         <v>0</v>
       </c>
-      <c r="AJ138">
-        <v>1</v>
-      </c>
       <c r="AK138" t="inlineStr">
         <is>
           <t>NA</t>
@@ -28277,9 +28262,6 @@
       </c>
       <c r="AZ138">
         <v>12</v>
-      </c>
-      <c r="BA138">
-        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="139">
@@ -29491,7 +29473,7 @@
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>Andrés Arauz;Yaku Pérez;Isidro Romero;Gustavo Larrea;Carlos Sagnay;Giovanni Andrade;Paúl Carrasco;Ximena Peña;Guillermo Lasso;Guillermo Celi;Lucio Gutiérrez;Xavier Hervas; César Montúfar;Gerson Almeida;Juan Fernando Velasco;Pedro José Freile</t>
+          <t>Andrés Arauz;Yaku Pérez;Isidro Romero;Gustavo Larrea;Carlos Sagnay;Giovanny Andrade;Paúl Carrasco;Ximena Peña;Guillermo Lasso;Guillermo Celi;Lucio Gutiérrez;Xavier Hervas; César Montúfar;Gerson Almeida;Juan Fernando Velasco;Pedro José Freile</t>
         </is>
       </c>
       <c r="Q145" t="inlineStr">
@@ -29708,7 +29690,7 @@
       </c>
       <c r="P146" t="inlineStr">
         <is>
-          <t>el primero: Isidro Romero;Gustavo Larrea;Carlos Sagnay;Giovanni Andrade;Paúl Carrasco;Ximena Peña;Guillermo Lasso; el segundo:  Guillermo Celi;Lucio Gutiérrez;Xavier Hervas; César Montúfar;Gerson Almeida;Juan Fernando Velasco;Pedro José Freile</t>
+          <t>el primero: Isidro Romero;Gustavo Larrea;Carlos Sagnay;Giovanny Andrade;Paúl Carrasco;Ximena Peña;Guillermo Lasso; el segundo:  Guillermo Celi;Lucio Gutiérrez;Xavier Hervas; César Montúfar;Gerson Almeida;Juan Fernando Velasco;Pedro José Freile</t>
         </is>
       </c>
       <c r="Q146" t="inlineStr">
@@ -32045,7 +32027,7 @@
       </c>
       <c r="Q159" t="inlineStr">
         <is>
-          <t>Luis Alberto Lacalle;José Pepe Mujica</t>
+          <t>Luis Alberto Lacalle Herrera;José Pepe Mujica</t>
         </is>
       </c>
       <c r="U159" t="inlineStr">
@@ -34618,7 +34600,7 @@
       </c>
       <c r="P174" t="inlineStr">
         <is>
-          <t>José Domingo Arias;Juan Carlos Navarro;Juan Carlos Valera;Genaro López;Juan Jované.</t>
+          <t>José Domingo Arias;Juan Carlos Navarro;Juan Carlos Varela;Genaro López;Juan Jované.</t>
         </is>
       </c>
       <c r="Q174" t="inlineStr">
@@ -35016,7 +34998,7 @@
       </c>
       <c r="P176" t="inlineStr">
         <is>
-          <t>Ana Matilde Gómez;Ricardo Lombana;Marco Ameglio;José Blandón;Saúl Méndez;Rómolo Rux</t>
+          <t>Ana Matilde Gómez;Ricardo Lombana;Marco Ameglio;José Isabel Blandón;Saúl Méndez;Rómolo Roux</t>
         </is>
       </c>
       <c r="Q176" t="inlineStr">
@@ -38151,7 +38133,7 @@
       </c>
       <c r="P193" t="inlineStr">
         <is>
-          <t>Gonzalo Sánchez de Losada;Manfred Reyes Villa</t>
+          <t>Gonzalo Sánchez de Lozada;Manfred Reyes Villa</t>
         </is>
       </c>
       <c r="Q193" t="inlineStr">
@@ -38345,7 +38327,7 @@
       </c>
       <c r="Q194" t="inlineStr">
         <is>
-          <t>René Blattmann, Nicolás Valdivia, Costa Obregón  y Rolando Morales, Felipe Quispe, Johnny Fernández ni Evo Morales</t>
+          <t>René Blattmann;Nicolás Valdivia;Costa Obregón;Rolando Morales;Felipe Quispe;Johnny Fernández;Evo Morales</t>
         </is>
       </c>
       <c r="R194" t="inlineStr">
@@ -38407,10 +38389,10 @@
         </is>
       </c>
       <c r="AI194">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AJ194">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AK194" t="inlineStr">
         <is>
@@ -38489,7 +38471,7 @@
         <v>11</v>
       </c>
       <c r="BA194">
-        <v>0.5454545454545454</v>
+        <v>1.090909090909091</v>
       </c>
     </row>
     <row r="195">
@@ -39137,7 +39119,7 @@
       </c>
       <c r="P198" t="inlineStr">
         <is>
-          <t>Carlos Mesa;Jorge Tuto Quiroga;Feliciano Mamani;María de la Cruz Bayá;Chi Hyun Yung</t>
+          <t>Carlos Mesa;Jorge Tuto Quiroga;Feliciano Mamani;María de la Cruz Bayá;Chi Hyun Chung</t>
         </is>
       </c>
       <c r="Q198" t="inlineStr">
@@ -41686,7 +41668,7 @@
       </c>
       <c r="P212" t="inlineStr">
         <is>
-          <t>Arzu;Portillo</t>
+          <t>Álvaro Arzu;Alfonso Portillo</t>
         </is>
       </c>
       <c r="Q212" t="inlineStr">
@@ -41958,7 +41940,7 @@
       </c>
       <c r="P215" t="inlineStr">
         <is>
-          <t>Eduardo Suger;Fritz García-Gallont;Alvaro Colom;Manuel Conde;Leonel Lopez Rodas</t>
+          <t>Eduardo Suger;Fritz García-Gallont;Alvaro Colom;Manuel Conde Orellana;Leonel Lopez Rodas</t>
         </is>
       </c>
       <c r="Q215" t="inlineStr">
@@ -42901,7 +42883,7 @@
       </c>
       <c r="P220" t="inlineStr">
         <is>
-          <t>Juan Gutiérrez;Eduardo Sugar;Adela de Torre;Harold Caballeros;Alejandro Diamatei;Patricia de Arzú;Otto Pérez Molina;Manuel Baldizón;Rigoberta Menchú</t>
+          <t>Juan Gutiérrez;Eduardo Suger;Adela de Torre;Harold Caballeros;Alejandro Giammattei;Patricia de Arzú;Otto Pérez Molina;Manuel Baldizón;Rigoberta Menchú</t>
         </is>
       </c>
       <c r="Q220" t="inlineStr">
@@ -43072,12 +43054,9 @@
           <t>Movimiento de Inmigrantes Guatemaltecos;Coalición Nacional de Migrantes;Sindicato Internacional de Trabajadores de Servicios</t>
         </is>
       </c>
-      <c r="O221">
-        <v>5</v>
-      </c>
       <c r="P221" t="inlineStr">
         <is>
-          <t>;;;;</t>
+          <t>sin datos</t>
         </is>
       </c>
       <c r="Q221" t="inlineStr">
@@ -44028,7 +44007,7 @@
       </c>
       <c r="P226" t="inlineStr">
         <is>
-          <t>Sandra Torres;Roberto González;Lizardo Sosa;Zuri Ríos;Jimmy Morales</t>
+          <t>Sandra Torres;Roberto González;Lizardo Sosa;Zury Ríos;Jimmy Morales</t>
         </is>
       </c>
       <c r="Q226" t="inlineStr">
@@ -44227,7 +44206,7 @@
       </c>
       <c r="P227" t="inlineStr">
         <is>
-          <t>El primero: Manuel Baldizón;Alejandro Giammattei;Mario David García;Luis Fernando Pérez;Zury Ríos;El segundo: Aníbal García;Roberto González;Jimmy Morales;Miguel Ángel Sandoval;Lizardo Sosa;El tercero: Sandra Torres;José López Camposeco;Juan Gutiérrez;Mario Amílcar Estrada</t>
+          <t>El primero: Manuel Baldizón;Alejandro Giammattei;Mario David García;Luis Fernando Pérez;Zury Ríos;El segundo: Aníbal García;Roberto González;Jimmy Morales;Miguel Ángel Sandoval;Lizardo Sosa;El tercero: Sandra Torres;José López Camposeco;Juan Gutiérrez;Mario Estrada</t>
         </is>
       </c>
       <c r="Q227" t="inlineStr">
@@ -44436,7 +44415,7 @@
       </c>
       <c r="P228" t="inlineStr">
         <is>
-          <t>Sandra Torres;Jimmy Morales; Aníbal García;Alejandro Giammattei;José Ángel López;Luis Fernando Pérez;Lizardo Sosa;Miguel Ángel Sandoval;Roberto González;x</t>
+          <t>Sandra Torres;Jimmy Morales; Aníbal García;Alejandro Giammattei;José Ángel López;Luis Fernando Pérez;Lizardo Sosa;Miguel Ángel Sandoval;Roberto González;sin datos</t>
         </is>
       </c>
       <c r="Q228" t="inlineStr">
@@ -45833,7 +45812,7 @@
       </c>
       <c r="P235" t="inlineStr">
         <is>
-          <t>José Luis Chea Urruela;Luis Velásquez;Fredy Cabrera;Aníbal García;(por el partido victoria está el candidato a la vicepresidencia)Erico Can</t>
+          <t>José Luis Chea Urruela;Luis Velásquez;Fredy Cabrera;Aníbal García;Erico Can</t>
         </is>
       </c>
       <c r="Q235" t="inlineStr">
@@ -46258,11 +46237,11 @@
         </is>
       </c>
       <c r="O237">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P237" t="inlineStr">
         <is>
-          <t>20 junio: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;12 junio: Armando Castillo;Amílcar PopXXXRivera;Álvaro Trujillo;Giulio Talamonti;31 mayo: Giovanni Reyes;Giulio Talamonti;Rudio Lecsan Mérida;30 mayo: Álvaro Trujillo;Amílcar Pop;Armando Castillo;29 mayo: Luis Lam;Julio Rivera Clavería;22 de mayo: Almícar Rivera Victoria;Manuel Villacorta;Ricardo Sagastume;18 de mayo: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;17 mayo: Rudio Lecsan Mérida;Giovanni Reyes;Giulio Talamonti;16 mayo: Álvaro Trujillo;Amílcar Pop;Armando Castillo;15 mayo: Julio Rivera Clavería;Luis Lam;Rudy Guzmán;4 mayo: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;27 abril: Sandra Torres;Edmond Mulet;Manuel Conde Orellana;</t>
+          <t>20 junio: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;12 junio: Armando Castillo;Amílcar Pop;Álvaro Trujillo;Giulio Talamonti;31 mayo: Giovanni Reyes;Giulio Talamonti;Rudio Lecsan Mérida;30 mayo: Álvaro Trujillo;Amílcar Pop;Armando Castillo;29 mayo: Luis Lam;Julio Rivera Clavería;22 de mayo: Amílcar Rivera Victoria;Manuel Villacorta;Ricardo Sagastume;18 de mayo: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;17 mayo: Rudio Lecsan Mérida;Giovanni Reyes;Giulio Talamonti;16 mayo: Álvaro Trujillo;Amílcar Pop;Armando Castillo;15 mayo: Julio Rivera Clavería;Luis Lam;Rudy Guzmán;4 mayo: Sandra Torres;Zury Ríos;Edmond Mulet;Manuel Conde Orellana;27 abril: Sandra Torres;Edmond Mulet;Manuel Conde Orellana</t>
         </is>
       </c>
       <c r="Q237" t="inlineStr">
@@ -46343,7 +46322,7 @@
         <v>3</v>
       </c>
       <c r="AJ237">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AK237" t="inlineStr">
         <is>
@@ -46422,7 +46401,7 @@
         <v>22</v>
       </c>
       <c r="BA237">
-        <v>1.954545454545455</v>
+        <v>1.909090909090909</v>
       </c>
     </row>
     <row r="238">
@@ -46474,7 +46453,7 @@
       </c>
       <c r="P238" t="inlineStr">
         <is>
-          <t>el primero: Francisco Arredondo;Geovanni Reyes;el segundo: Bernardo Arévalo;Luis Lam;el tercero: Ricardo Sagastume;Hugo Peña;Giulio Talamonti;Julio Rivera Clavería</t>
+          <t>el primero: Francisco Arredondo;Giovanni Reyes;el segundo: Bernardo Arévalo;Luis Lam;el tercero: Ricardo Sagastume;Hugo Peña;Giulio Talamonti;Julio Rivera Clavería</t>
         </is>
       </c>
       <c r="Q238" t="inlineStr">
@@ -47870,7 +47849,7 @@
       </c>
       <c r="Q245" t="inlineStr">
         <is>
-          <t>Sandra Torres;Zury Ríos;Edmond Mulet;Bernardo Arévalo;Manuel Conde Orellana;Amílcar Rivera;Manuel Villacorta;Luis Lam;Samuel Morales;Rudy Guzmán;Giulio Talamonti;Almícar Pop;Julio Rivera Clavería;Rudio Lecsan Mérida;Isaac Farchi;Ricardo Sagastume</t>
+          <t>Sandra Torres;Zury Ríos;Edmond Mulet;Bernardo Arévalo;Manuel Conde Orellana;Amílcar Rivera;Manuel Villacorta;Luis Lam;Samuel Morales;Rudy Guzmán;Giulio Talamonti;Amílcar Pop;Julio Rivera Clavería;Rudio Lecsan Mérida;Isaac Farchi;Ricardo Sagastume</t>
         </is>
       </c>
       <c r="U245" t="inlineStr">
@@ -48911,7 +48890,7 @@
       </c>
       <c r="P251" t="inlineStr">
         <is>
-          <t>Orle Aníbal Solís;Romeo Vázquez Velázquez;Mauricio Villeda Bermúdez;Salvador Nasralla;Iris Xiomara Castro de Zelaya;Jorge Rafael Aguilar;Andrés Pavón Murillo;Juan Orlando Hernández</t>
+          <t>Orle Aníbal Solís;Romeo Vásquez Velázquez;Mauricio Villeda Bermúdez;Salvador Nasralla;Iris Xiomara Castro de Zelaya;Jorge Rafael Aguilar;Andrés Pavón Murillo;Juan Orlando Hernández</t>
         </is>
       </c>
       <c r="Q251" t="inlineStr">
@@ -49122,7 +49101,7 @@
       </c>
       <c r="P252" t="inlineStr">
         <is>
-          <t>José Alfonso Díaz Narváez;Salvador Nasralla;Eliseo Vallecillo Reyes;Lucas Evangelisto Aguilera;Luis Orlando Zelaya;Romeo Orlando Vásquez Velásquez;Isaías Fonseca Aguilar</t>
+          <t>José Alfonso Díaz Narváez;Salvador Nasralla;Eliseo Vallecillo Reyes;Lucas Evangelisto Aguilera;Luis Orlando Zelaya;Romeo Vásquez Velásquez;Isaías Fonseca Aguilar</t>
         </is>
       </c>
       <c r="Q252" t="inlineStr">
@@ -50538,7 +50517,7 @@
       </c>
       <c r="P259" t="inlineStr">
         <is>
-          <t>Álvaro Uribe Vélez;Noemí Sanín Posada;Luis Eduardo Garzón;Horacio Serpa Uribe</t>
+          <t>Álvaro Uribe Vélez;Noemí Sanín;Luis Eduardo Garzón;Horacio Serpa</t>
         </is>
       </c>
       <c r="Q259" t="inlineStr">
@@ -52183,7 +52162,7 @@
       </c>
       <c r="P268" t="inlineStr">
         <is>
-          <t>Gustavo Petro;Germán Vargas;Noemí Sanín;Juan Manuel Santos;Rafael Pardo;Antanas Mockus</t>
+          <t>Gustavo Petro;Germán Vargas Lleras;Noemí Sanín;Juan Manuel Santos;Rafael Pardo;Antanas Mockus</t>
         </is>
       </c>
       <c r="Q268" t="inlineStr">
@@ -55224,7 +55203,7 @@
       </c>
       <c r="P284" t="inlineStr">
         <is>
-          <t>Humberto De La Calle;Gustavo Petro;Sergio Fajardo</t>
+          <t>Humberto de la Calle;Gustavo Petro;Sergio Fajardo</t>
         </is>
       </c>
       <c r="Q284" t="inlineStr">
@@ -55423,7 +55402,7 @@
       </c>
       <c r="P285" t="inlineStr">
         <is>
-          <t>Gustavo Petro;Iván Duque;Germán Vargas Lleras;Humberto De la Calle</t>
+          <t>Gustavo Petro;Iván Duque;Germán Vargas Lleras;Humberto de la Calle</t>
         </is>
       </c>
       <c r="Q285" t="inlineStr">
@@ -55847,7 +55826,7 @@
       </c>
       <c r="P287" t="inlineStr">
         <is>
-          <t>Humberto De la Calle;Sergio Fajardo;Iván Duque;Germán Vargas</t>
+          <t>Humberto de la Calle;Sergio Fajardo;Iván Duque;Germán Vargas</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -56263,7 +56242,7 @@
       </c>
       <c r="Q289" t="inlineStr">
         <is>
-          <t>Humberto de la Calle Lombana</t>
+          <t>Humberto de la Calle</t>
         </is>
       </c>
       <c r="S289">
@@ -59448,7 +59427,7 @@
       </c>
       <c r="P304" t="inlineStr">
         <is>
-          <t>Ingrid Batancourt;Sergio Fajardo;John Milton Rodríguez;Federico Gutiérrez;Enrique Gómez;Luis Pérez</t>
+          <t>Ingrid Betancourt;Sergio Fajardo;John Milton Rodríguez;Federico Gutiérrez;Enrique Gómez;Luis Pérez</t>
         </is>
       </c>
       <c r="Q304" t="inlineStr">
@@ -59658,7 +59637,7 @@
       </c>
       <c r="P305" t="inlineStr">
         <is>
-          <t>Rodolfo Hernández;Ingrid Batancourt;John Milton Rodríguez;Federico Gutiérrez;Enrique Gómez;Luis Pérez</t>
+          <t>Rodolfo Hernández;Ingrid Betancourt;John Milton Rodríguez;Federico Gutiérrez;Enrique Gómez;Luis Pérez</t>
         </is>
       </c>
       <c r="Q305" t="inlineStr">
@@ -60113,7 +60092,7 @@
       </c>
       <c r="P307" t="inlineStr">
         <is>
-          <t>Ingrid Batancourt;John Milton Rodríguez</t>
+          <t>Ingrid Betancourt;John Milton Rodríguez</t>
         </is>
       </c>
       <c r="Q307" t="inlineStr">
@@ -60783,7 +60762,7 @@
       </c>
       <c r="P310" t="inlineStr">
         <is>
-          <t>Enrique Gómez;Rodolfo Hernández;Ingrid Batancourt;John Milton Rodríguez;Federico Gutiérrez;Sergio Fajardo</t>
+          <t>Enrique Gómez;Rodolfo Hernández;Ingrid Betancourt;John Milton Rodríguez;Federico Gutiérrez;Sergio Fajardo</t>
         </is>
       </c>
       <c r="Q310" t="inlineStr">
@@ -61693,7 +61672,7 @@
       </c>
       <c r="Q314" t="inlineStr">
         <is>
-          <t>Gustavo Petro;Sergio Fajardo;Ingrid Bentacourt;Luis Pérez</t>
+          <t>Gustavo Petro;Sergio Fajardo;Ingrid Betancourt;Luis Pérez</t>
         </is>
       </c>
       <c r="R314" t="inlineStr">
@@ -63809,7 +63788,7 @@
       </c>
       <c r="P326" t="inlineStr">
         <is>
-          <t>Rolando Araya Monge;Otto Guevara;Abel Pacheco de la Espriella;Ottón Solís</t>
+          <t>Rolando Araya;Otto Guevara;Abel Pacheco de la Espriella;Ottón Solís</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -64016,7 +63995,7 @@
       </c>
       <c r="P327" t="inlineStr">
         <is>
-          <t>Abel Pacheco de la Espriella;Rolando Araya Monge</t>
+          <t>Abel Pacheco de la Espriella;Rolando Araya</t>
         </is>
       </c>
       <c r="Q327" t="inlineStr">
@@ -64223,7 +64202,7 @@
       </c>
       <c r="P328" t="inlineStr">
         <is>
-          <t>Abel Pacheco de la Espriella;Rolando Araya Monge</t>
+          <t>Abel Pacheco de la Espriella;Rolando Araya</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -64415,7 +64394,7 @@
       </c>
       <c r="P329" t="inlineStr">
         <is>
-          <t>Abel Pacheco de la Espriella;Rolando Araya Monge</t>
+          <t>Abel Pacheco de la Espriella;Rolando Araya</t>
         </is>
       </c>
       <c r="Q329" t="inlineStr">
@@ -64622,7 +64601,7 @@
       </c>
       <c r="P330" t="inlineStr">
         <is>
-          <t>primera:  Humberto Arce;Ottón Solís;Otto Guevara;segunda: Abel Pacheco de la Espirella;Álvaro Montero;Ricardo Toledo;tercera: Vladimir de la Cruz de Lemos;Bolívar Serrano Hidalgo;José Manuel Echandi Meza;cuarta:  Antonio Álvarez Desanti;Walter Muñoz Céspedes;Juan José Vargas Fallas;José Miguel Villalobos Umaña</t>
+          <t>primera: Humberto Arce;Ottón Solís;Otto Guevara;segunda: Abel Pacheco de la Espirella;Álvaro Montero;Ricardo Toledo;tercera: Vladimir de la Cruz de Lemos;Bolívar Serrano Hidalgo;José Manuel Echandi;cuarta:  Antonio Álvarez Desanti;Walter Muñoz;Juan José Vargas Fallas;José Miguel Villalobos</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -64831,7 +64810,7 @@
       </c>
       <c r="P331" t="inlineStr">
         <is>
-          <t>en el primero: Juan José Vargas;Álvaro Montero;Bolívar Serrano;José Miguel Villalobos;Humberto Vargas;en el segundo: Ottón Solís;Otto Guevara;Óscar Arias;Antonio Álvarez;Ricardo Toledo;en el tercero: José Manuel Echandi;Humberto Arce;Wálter Muñoz;Vladimir de la Cruz</t>
+          <t>en el primero: Juan José Vargas;Álvaro Montero;Bolívar Serrano Hidalgo;José Miguel Villalobos;Humberto Vargas;en el segundo: Ottón Solís;Otto Guevara;Óscar Arias;Antonio Álvarez Desanti;Ricardo Toledo;en el tercero: José Manuel Echandi;Humberto Arce;Wálter Muñoz;Vladimir de la Cruz</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -65025,7 +65004,7 @@
       </c>
       <c r="P332" t="inlineStr">
         <is>
-          <t>primero: Carlos Alvarado Quesada;Otto Guevara;Edgardo Araya;Mario Redondo Poveda;Rodolfo Hernández Gómez;Antonio Álvarez Desanti; segundo: Fabricio Alvarado;Oscar López;Sergio Mena;John Vega</t>
+          <t>primero: Carlos Alvarado Quesada;Otto Guevara;Edgardo Araya;Mario Redondo Poveda;Rodolfo Hernández;Antonio Álvarez Desanti; segundo: Fabricio Alvarado Muñoz;Oscar López;Sergio Mena;Jhon Vega</t>
         </is>
       </c>
       <c r="Q332" t="inlineStr">
@@ -66062,12 +66041,12 @@
       </c>
       <c r="P337" t="inlineStr">
         <is>
-          <t>primero: Johnny Araya;José Miguel Corrales;Otto Guevara;Rodolfo Piza;Luis Guillermo Solís;José María Villalta; segundo: José Manuel Echandi;Héctor Monestel;Sergio Mena</t>
+          <t>primero: Johnny Araya;José Miguel Corrales Bolaños;Otto Guevara;Rodolfo Piza;Luis Guillermo Solís;José María Villalta; segundo: José Manuel Echandi;Héctor Monestel;Sergio Mena</t>
         </is>
       </c>
       <c r="Q337" t="inlineStr">
         <is>
-          <t>Carlos Luis Avendaño;Oscar López;Walter Muñoz; Justo Orozco</t>
+          <t>Carlos Avendaño;Oscar López;Walter Muñoz; Justo Orozco</t>
         </is>
       </c>
       <c r="R337" t="inlineStr">
@@ -66269,7 +66248,7 @@
       </c>
       <c r="P338" t="inlineStr">
         <is>
-          <t>primer bloque: Sergio Mena;José Miguel Corrales;Oscar López;Héctor Monestel;segundo bloque: Otto Guevara;Rodolfo Piza;Luis Guillermo Solis;Jose María Villalta</t>
+          <t>primer bloque: Sergio Mena;José Miguel Corrales Bolaños;Oscar López;Héctor Monestel;segundo bloque: Otto Guevara;Rodolfo Piza;Luis Guillermo Solis;Jose María Villalta</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -66468,7 +66447,7 @@
       </c>
       <c r="P339" t="inlineStr">
         <is>
-          <t>primero: Hector Menestel Herrera;Jose Miguel Corrales Bolaños;Luis Guillermo Solís Rivera;Carlos Avendaño Carlo;Otto Guevara;Walter Muñoz Céspedes;segundo: Óscar López;José María Villalta; José Manuel Echandi;Johnny Araya;Justo Orozco;Rodolfo Piza;Sergio Mena</t>
+          <t>primero: Hector Menestel Herrera;Jose Miguel Corrales Bolaños;Luis Guillermo Solís;Carlos Avendaño;Otto Guevara;Walter Muñoz;segundo: Óscar López;José María Villalta; José Manuel Echandi;Johnny Araya;Justo Orozco;Rodolfo Piza;Sergio Mena</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -67249,7 +67228,7 @@
       </c>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Luis Guillermo Solís;José María Villata;Rodolfo Jhonny Araya;Otto Guevara;Piza</t>
+          <t>Luis Guillermo Solís;José María Villalta;Rodolfo Jhonny Araya;Otto Guevara;Rodolfo Piza</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -67658,7 +67637,7 @@
       </c>
       <c r="P345" t="inlineStr">
         <is>
-          <t>Luis Guillermo Solís;José María Villalta;José Miguel Corrales;Otto Guevara</t>
+          <t>Luis Guillermo Solís;José María Villalta;José Miguel Corrales Bolaños;Otto Guevara</t>
         </is>
       </c>
       <c r="Q345" t="inlineStr">
@@ -67858,16 +67837,16 @@
         </is>
       </c>
       <c r="O346">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P346" t="inlineStr">
         <is>
-          <t>Héctor Monestel;José Miguel Corales;Walter Muñoz;Óscar López;José María Villalta;José Manuel Echandi;Justo Orozco;Sergio Mena</t>
+          <t>Héctor Monestel;Walter Muñoz;Óscar López;José María Villalta;José Manuel Echandi;Justo Orozco;Sergio Mena</t>
         </is>
       </c>
       <c r="Q346" t="inlineStr">
         <is>
-          <t>José Miguel Corrales;Héctor Monestel;José Manuel Echandi;Walter Muñoz;Sergio Mena</t>
+          <t>José Miguel Corrales Bolaños;Héctor Monestel;José Manuel Echandi;Walter Muñoz;Sergio Mena</t>
         </is>
       </c>
       <c r="U346" t="inlineStr">
@@ -67925,7 +67904,7 @@
         <v>5</v>
       </c>
       <c r="AJ346">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AK346" t="inlineStr">
         <is>
@@ -68004,7 +67983,7 @@
         <v>13</v>
       </c>
       <c r="BA346">
-        <v>1</v>
+        <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="347">
@@ -68056,12 +68035,12 @@
       </c>
       <c r="P347" t="inlineStr">
         <is>
-          <t>primer bloque: Carlos Alvarado;Otto Guevara;Rodolfo Hernández;Stephanie Campos;Mario Redondo; segundo bloque:  Jhon Vega;Edgardo Araya;Sergio Mena</t>
+          <t>primer bloque: Carlos Alvarado Quesada;Otto Guevara;Rodolfo Hernández;Stephanie Campos;Mario Redondo Poveda; segundo bloque: Jhon Vega;Edgardo Araya;Sergio Mena</t>
         </is>
       </c>
       <c r="Q347" t="inlineStr">
         <is>
-          <t>Antonio Álvarez Desanti;Óscar López;Fabricio Alvarado;Rodolfo Piza;Juan Diego Castro</t>
+          <t>Antonio Álvarez Desanti;Óscar López;Fabricio Alvarado Muñoz;Rodolfo Piza;Juan Diego Castro</t>
         </is>
       </c>
       <c r="U347" t="inlineStr">
@@ -68260,12 +68239,12 @@
       </c>
       <c r="P348" t="inlineStr">
         <is>
-          <t>Antonio Álvarez Desanti;Sergio Mena;John Vega;Óscar López;Carlos Alvarado;Rodolfo Hernández;Fabricio Alvarado</t>
+          <t>Antonio Álvarez Desanti;Sergio Mena;Jhon Vega;Óscar López;Carlos Alvarado Quesada;Rodolfo Hernández;Fabricio Alvarado</t>
         </is>
       </c>
       <c r="Q348" t="inlineStr">
         <is>
-          <t>Mario Redondo;Otto Guevara;Rodolfo Piza;Juan Diego Castro</t>
+          <t>Mario Redondo Poveda;Otto Guevara;Rodolfo Piza;Juan Diego Castro</t>
         </is>
       </c>
       <c r="U348" t="inlineStr">
@@ -68464,7 +68443,7 @@
       </c>
       <c r="P349" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q349" t="inlineStr">
@@ -68668,7 +68647,7 @@
       </c>
       <c r="P350" t="inlineStr">
         <is>
-          <t>primero: Mario Redondo Poveda;Oscar López;Edgardo Araya;Juan Diego Castro Fernández;Antonio Álvarez Desanti;Sergio Mena Díaz;Fabricio Alvarado; segundo: Rodolfo Hernández;Carlos Alvarado Quesada;Jhon Vega;Rodolfo Piza;Otto Guevara Guth;Stephanie Campos Arrieta</t>
+          <t>primero: Mario Redondo Poveda;Oscar López;Edgardo Araya;Juan Diego Castro Fernández;Antonio Álvarez Desanti;Sergio Mena;Fabricio Alvarado Muñoz; segundo: Rodolfo Hernández;Carlos Alvarado Quesada;Jhon Vega;Rodolfo Piza;Otto Guevara;Stephanie Campos</t>
         </is>
       </c>
       <c r="Q350" t="inlineStr">
@@ -68875,7 +68854,7 @@
       </c>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q351" t="inlineStr">
@@ -69074,7 +69053,7 @@
       </c>
       <c r="P352" t="inlineStr">
         <is>
-          <t>Carlos Alvarado Quesada;Juan Diego Castro Fernández;Antonio Álvarez Desanti;Rodolfo Hernández Gómez;Fabricio Alvarado Muñoz;Rodolfo Piza Rocafort</t>
+          <t>Carlos Alvarado Quesada;Juan Diego Castro Fernández;Antonio Álvarez Desanti;Rodolfo Hernández;Fabricio Alvarado Muñoz;Rodolfo Piza Rocafort</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -69268,7 +69247,7 @@
       </c>
       <c r="P353" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -69631,7 +69610,7 @@
       </c>
       <c r="P355" t="inlineStr">
         <is>
-          <t>Stephanie Campos Arrieta;Mario Redondo Poveda;Jhon Vega;Edgardo Araya;Oscar López;Otto Guevara;Sergio Mena Díaz</t>
+          <t>Stephanie Campos;Mario Redondo Poveda;Jhon Vega;Edgardo Araya;Oscar López;Otto Guevara;Sergio Mena</t>
         </is>
       </c>
       <c r="Q355" t="inlineStr">
@@ -69833,7 +69812,7 @@
       </c>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Carlos Alvarado;Rodolfo Piza;Juan Diego Castro;Antonio Álvarez Desanti;Fabricio Alvarado</t>
+          <t>Carlos Alvarado Quesada;Rodolfo Piza;Juan Diego Castro Fernández;Antonio Álvarez Desanti;Fabricio Alvarado</t>
         </is>
       </c>
       <c r="Q356" t="inlineStr">
@@ -70042,7 +70021,7 @@
       </c>
       <c r="P357" t="inlineStr">
         <is>
-          <t>Rodolfo Piza;Fabricio Alvarado;Antonio Álvarez Desanti;Edgardo Araya;Rodolfo Hernández;Juan Diego Castro</t>
+          <t>Rodolfo Piza;Fabricio Alvarado Muñoz;Antonio Álvarez Desanti;Edgardo Araya;Rodolfo Hernández;Juan Diego Castro</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -70259,7 +70238,7 @@
       </c>
       <c r="P358" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q358" t="inlineStr">
@@ -70468,7 +70447,7 @@
       </c>
       <c r="P359" t="inlineStr">
         <is>
-          <t>primero: Carlos Alvarado Quesada;Antonio Álvarez Desanti;Edgardo Araya Sibaja; segundo:  Jhonn Vega Masis;Stephanie Campos Arrieta;Rodolfo Hernández Gómez;Sergio Mena Díaz;Mario Redondo Poveda</t>
+          <t>primero: Carlos Alvarado Quesada;Antonio Álvarez Desanti;Edgardo Araya; segundo: Jhon Vega;Stephanie Campos;Rodolfo Hernández;Sergio Mena;Mario Redondo Poveda</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -70685,7 +70664,7 @@
       </c>
       <c r="P360" t="inlineStr">
         <is>
-          <t>Edgardo Araya;Carlos Alvarado;Antonio Álvarez Desanti;Juan Diego Castro;Otto Guevara;Rodolfo Piza</t>
+          <t>Edgardo Araya;Carlos Alvarado Quesada;Antonio Álvarez Desanti;Juan Diego Castro Fernández;Otto Guevara;Rodolfo Piza</t>
         </is>
       </c>
       <c r="Q360" t="inlineStr">
@@ -70887,12 +70866,12 @@
       </c>
       <c r="P361" t="inlineStr">
         <is>
-          <t>Carlos Alvarado Quesada;Mario Redondo Poveda;Jhonn Vega Masis;Sergio Mena Díaz;Oscar López;Otto Guevara;Edgardo Araya;Stephanie Campos Arrieta;Fabricio Alvarado</t>
+          <t>Carlos Alvarado Quesada;Mario Redondo Poveda;Jhon Vega;Sergio Mena;Oscar López;Otto Guevara;Edgardo Araya;Stephanie Campos;Fabricio Alvarado</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
         <is>
-          <t>Antonio Álvarez Desanti;Rodolfo Piza;Juan Diego Castro;Rodolfo Hernández</t>
+          <t>Antonio Álvarez Desanti;Rodolfo Piza;Juan Diego Castro Fernández;Rodolfo Hernández</t>
         </is>
       </c>
       <c r="S361">
@@ -71084,7 +71063,7 @@
       </c>
       <c r="P362" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q362" t="inlineStr">
@@ -71281,7 +71260,7 @@
       </c>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada;Antonio Álvarez Desanti;Juan Diego Castro;Rodolfo Hernández;Rodolfo Piza</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada;Antonio Álvarez Desanti;Juan Diego Castro Fernández;Rodolfo Hernández;Rodolfo Piza</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
@@ -71478,7 +71457,7 @@
       </c>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -71680,7 +71659,7 @@
       </c>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Carlos Alvarado Quesada;Antonio Álvarez De Santis;Edgardo Araya;Mario Arredondo;Otto Guevara</t>
+          <t>Carlos Alvarado Quesada;Antonio Álvarez Desanti;Edgardo Araya;Mario Redondo Poveda;Otto Guevara</t>
         </is>
       </c>
       <c r="Q365" t="inlineStr">
@@ -71882,7 +71861,7 @@
       </c>
       <c r="P366" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -72086,7 +72065,7 @@
       </c>
       <c r="P367" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q367" t="inlineStr">
@@ -72305,7 +72284,7 @@
       </c>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Fabricio Alvarado;Carlos Alvarado Quesada</t>
+          <t>Fabricio Alvarado Muñoz;Carlos Alvarado Quesada</t>
         </is>
       </c>
       <c r="Q368" t="inlineStr">
@@ -72524,7 +72503,7 @@
       </c>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Carlos Alvarado Quesada;Rodolfo Hernández;Otto Guevara;Fabricio Alvarado;Edgardo Araya</t>
+          <t>Carlos Alvarado Quesada;Rodolfo Hernández;Otto Guevara;Fabricio Alvarado Muñoz;Edgardo Araya</t>
         </is>
       </c>
       <c r="Q369" t="inlineStr">
@@ -72730,7 +72709,7 @@
       </c>
       <c r="P370" t="inlineStr">
         <is>
-          <t>el primero: Rodrigo Chaves;Walter Muñoz;Welmer Ramos;Christian Rivera;eJosé María Villalta;Rodolfo Piza; el segundo: Oscar Campos;Luis Alberto Cordero Arias;Natalia Díaz;Rodolfo Hernández;Oscar López;Federico Malavassi;Sergio Mena;Jhon Vega; el tercero: Eduardo Cruickshank;Grevin Moya;Roulan Jiménez;Eliecer Feinzaig; Carmen Quesada;Martín Chinchilla;Maricela Morales</t>
+          <t>el primero: Rodrigo Chaves;Walter Muñoz;Welmer Ramos;Christian Rivera;eJosé María Villalta;Rodolfo Piza; el segundo: Oscar Campos;Luis Alberto Cordero;Natalia Díaz;Rodolfo Hernández;Oscar López;Federico Malavassi;Sergio Mena;Jhon Vega; el tercero: Eduardo Cruickshank;Greivin Moya;Roulan Jiménez;Eliecer Feinzaig; Carmen Quesada;Martín Chinchilla;Maricela Morales</t>
         </is>
       </c>
       <c r="Q370" t="inlineStr">
@@ -73385,7 +73364,7 @@
       </c>
       <c r="P373" t="inlineStr">
         <is>
-          <t>José María Villalta;Eli Feinzaig;Rodolfo Hernández</t>
+          <t>José María Villalta;Eliecer Feinzaig;Rodolfo Hernández</t>
         </is>
       </c>
       <c r="Q373" t="inlineStr">
@@ -73596,7 +73575,7 @@
       </c>
       <c r="P374" t="inlineStr">
         <is>
-          <t>el primero: Welmer Ramos;Fabricio Alvarado Muñoz;Federico Malavassi;Carmen Quesada;Grevin Moya;Martín Chinchilla; segundo: Lineth Saborío;Rodolfo Hernández;Luis Alberto Cordero;Eduardo Cruickshank;Rodrigo Chaves;Eliecer Feinzaig; el tercero: Christian Rivera;Maricela Morales;Roulan Jiménez;Sergio Mena;Rolando Araya;Oscar López; el cuarto:      Natalia Díaz;José María Figueres;Oscar Campos;Walter Muñoz;Rodolfo Piza;Jhon Vega;José María Villalta</t>
+          <t>el primero: Welmer Ramos;Fabricio Alvarado Muñoz;Federico Malavassi;Carmen Quesada;Greivin Moya;Martín Chinchilla; segundo: Lineth Saborío;Rodolfo Hernández;Luis Alberto Cordero;Eduardo Cruickshank;Rodrigo Chaves;Eliecer Feinzaig; el tercero: Christian Rivera;Maricela Morales;Roulan Jiménez;Sergio Mena;Rolando Araya;Oscar López; el cuarto: Natalia Díaz;José María Figueres;Oscar Campos;Walter Muñoz;Rodolfo Piza;Jhon Vega;José María Villalta</t>
         </is>
       </c>
       <c r="Q374" t="inlineStr">
@@ -74460,12 +74439,12 @@
       </c>
       <c r="P378" t="inlineStr">
         <is>
-          <t>el primero:  Welmer Ramos;Federico Malavassi;Carmen Quesada;Martín Chinchilla; el segundo: Eliecer Feinzaig;Christian Rivera;Roulan Jiménez;Sergio Mena;Rodrigo Chaves; el tercero: John Vega</t>
+          <t>el primero:  Welmer Ramos;Federico Malavassi;Carmen Quesada;Martín Chinchilla; el segundo: Eliecer Feinzaig;Christian Rivera;Roulan Jiménez;Sergio Mena;Rodrigo Chaves; el tercero: Jhon Vega</t>
         </is>
       </c>
       <c r="Q378" t="inlineStr">
         <is>
-          <t>al primero: Fabricio Alvarado Muñoz;Greivin Moya;Lineth Saborío;Rodlfo Hernández; al segundo: Luis Alberto Cordero;Eduardo Cruickshank;Maricela Morales; al tercero: Rolando Araya;Oscar López;Natalia Díaz;José María Figueres;Oscar Campos;Walter Muñoz;Rodolfo Piza;José María Villalta</t>
+          <t>al primero: Fabricio Alvarado Muñoz;Greivin Moya;Lineth Saborío;Rodolfo Hernández; al segundo: Luis Alberto Cordero;Eduardo Cruickshank;Maricela Morales; al tercero: Rolando Araya;Oscar López;Natalia Díaz;José María Figueres;Oscar Campos;Walter Muñoz;Rodolfo Piza;José María Villalta</t>
         </is>
       </c>
       <c r="R378" t="inlineStr">
@@ -74915,7 +74894,7 @@
       </c>
       <c r="P380" t="inlineStr">
         <is>
-          <t>el primero: Federico Malavassi;Gerardo Chaves;Sergio Mena;Christian Rivera;Roulan Jiménez;Oscar Campos;Walter Quesada;Gabriela San Román; el segundo: John Vega;Maricela Morales;Sebastián Urbina;Ana Lupita Mora;Vanessa Calvo</t>
+          <t>el primero: Federico Malavassi;Gerardo Chaves;Sergio Mena;Christian Rivera;Roulan Jiménez;Oscar Campos;Walter Quesada;Gabriela San Román; el segundo: Jhon Vega;Maricela Morales;Sebastián Urbina;Ana Lupita Mora;Vanessa Calvo</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -77477,7 +77456,7 @@
       </c>
       <c r="P392" t="inlineStr">
         <is>
-          <t>Parker;Guardado;Zamora;García</t>
+          <t>Rodolfo Parker;FacundoGuardado;Rubén Zamora;Salvador Néstor García</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">

</xml_diff>

<commit_message>
commit avances en creacion de base de datos una eleccion una fila
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_final1v2023.xlsx
+++ b/tesis_doctorado/datav2023/base_final1v2023.xlsx
@@ -14518,7 +14518,7 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami ;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
+          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
@@ -27037,7 +27037,7 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>Horacio Cartes; Efraín Alegre; Miguel Carrizosa; Mario Ferreiro</t>
+          <t>Horacio Cartes; Efraín Alegre; Miguel Carrizosa;Mario Ferreiro</t>
         </is>
       </c>
       <c r="Q129" t="inlineStr">
@@ -27248,7 +27248,7 @@
       </c>
       <c r="P130" t="inlineStr">
         <is>
-          <t>Horacio Cartes; Efraín Alegre; Miguel Carrizosa; Mario Ferreiro</t>
+          <t>Horacio Cartes; Efraín Alegre; Miguel Carrizosa;Mario Ferreiro</t>
         </is>
       </c>
       <c r="Q130" t="inlineStr">
@@ -27454,7 +27454,7 @@
       </c>
       <c r="P131" t="inlineStr">
         <is>
-          <t>Efraín Alegre; Miguel Carrizosa; Mario Ferreiro; Lino Oviedo; Aníbal Carrillo</t>
+          <t>Efraín Alegre;Miguel Carrizosa;Mario Ferreiro;Lino Oviedo;Aníbal Carrillo</t>
         </is>
       </c>
       <c r="Q131" t="inlineStr">
@@ -55088,7 +55088,7 @@
         </is>
       </c>
       <c r="AY279">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ279">
         <v>6</v>
@@ -55296,7 +55296,7 @@
         </is>
       </c>
       <c r="AY280">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ280">
         <v>6</v>
@@ -55507,7 +55507,7 @@
         </is>
       </c>
       <c r="AY281">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ281">
         <v>6</v>
@@ -55716,7 +55716,7 @@
         </is>
       </c>
       <c r="AY282">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ282">
         <v>6</v>
@@ -55940,7 +55940,7 @@
         </is>
       </c>
       <c r="AY283">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ283">
         <v>6</v>
@@ -56161,7 +56161,7 @@
         </is>
       </c>
       <c r="AY284">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ284">
         <v>6</v>
@@ -56370,7 +56370,7 @@
         </is>
       </c>
       <c r="AY285">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ285">
         <v>6</v>
@@ -56579,7 +56579,7 @@
         </is>
       </c>
       <c r="AY286">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ286">
         <v>6</v>
@@ -56788,7 +56788,7 @@
         </is>
       </c>
       <c r="AY287">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ287">
         <v>6</v>
@@ -57002,7 +57002,7 @@
         </is>
       </c>
       <c r="AY288">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ288">
         <v>6</v>
@@ -57211,7 +57211,7 @@
         </is>
       </c>
       <c r="AY289">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ289">
         <v>6</v>
@@ -57425,7 +57425,7 @@
         </is>
       </c>
       <c r="AY290">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ290">
         <v>6</v>
@@ -57641,7 +57641,7 @@
         </is>
       </c>
       <c r="AY291">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ291">
         <v>6</v>
@@ -57850,7 +57850,7 @@
         </is>
       </c>
       <c r="AY292">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ292">
         <v>6</v>
@@ -58069,7 +58069,7 @@
         </is>
       </c>
       <c r="AY293">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ293">
         <v>6</v>
@@ -58292,7 +58292,7 @@
         </is>
       </c>
       <c r="AY294">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ294">
         <v>6</v>

</xml_diff>

<commit_message>
cree base de encuestas y base de candidatos de nuevo
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_final1v2023.xlsx
+++ b/tesis_doctorado/datav2023/base_final1v2023.xlsx
@@ -12495,7 +12495,7 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Hernán Büchi Buc;Patricio Aylwin Azócar</t>
+          <t>Hernán Büchi;Patricio Aylwin Azócar</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
@@ -23162,7 +23162,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>Keiko Fujimori Higuchi;Óscar Oscar Luis Castañeda Lossio;Pedro Pablo Kuczynski;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Reymer Rodríguez;Humberto Pinazo Bella;Rafael Belaúnde Aubry;José Manuel Rodríguez Cuadros;Ricardo Noriega Salaverry;José Antonio Ñique de la Puente</t>
+          <t>Keiko Fujimori Higuchi;Oscar Luis Castañeda Lossio;Pedro Pablo Kuczynski;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Reymer Rodríguez;Humberto Pinazo Bella;Rafael Belaúnde Aubry;José Manuel Rodríguez Cuadros;Ricardo Noriega Salaverry;José Antonio Ñique de la Puente</t>
         </is>
       </c>
       <c r="Q110" t="inlineStr">
@@ -27037,7 +27037,7 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>Horacio Cartes; Efraín Alegre; Miguel Carrizosa;Mario Ferreiro</t>
+          <t>Horacio Cartes; Efraín Alegre;Miguel Carrizosa;Mario Ferreiro</t>
         </is>
       </c>
       <c r="Q129" t="inlineStr">

</xml_diff>

<commit_message>
rerun de cosas, creacion de primeros indicadores de nivel candidatos
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_final1v2023.xlsx
+++ b/tesis_doctorado/datav2023/base_final1v2023.xlsx
@@ -23202,7 +23202,7 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Keiko Fujimori Higuchi;Oscar Luis Castañeda Lossio;Pedro Pablo Kuczynski;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Reymer Rodríguez;Humberto Pinazo Bella;Rafael Belaúnde Aubry;José Manuel Rodríguez Cuadros;Ricardo Noriega Salaverry;José Antonio Ñique de la Puente</t>
+          <t>Keiko Fujimori Higuchi;Oscar Luis Castañeda Lossio;Pedro Pablo Kuczynski;Ollanta Moisés Humala Tasso;Alejandro Toledo Manrique;Juliana Reymer Rodríguez;Humberto Pinazo Bella;Rafael Belaúnde Aubry;Jose Manuel Rodriguez Cuadros;Ricardo Noriega Salaverry;Jose Nique de la Puente</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
@@ -23408,7 +23408,7 @@
       </c>
       <c r="P112" t="inlineStr">
         <is>
-          <t>Ollanta Moisés Humala Tasso;Ricardo Noriega Salaverry;Juliana Reymer Rodríguez;Manuel Rodríguez Cuadros;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;José Ñique de la Puente;Pedro Pablo Kuczynski;Humberto Pinazo Bella;Rafael Belaúnde Aubry;Oscar Luis Castañeda Lossio</t>
+          <t>Ollanta Moisés Humala Tasso;Ricardo Noriega Salaverry;Juliana Reymer Rodríguez;Jose Manuel Rodriguez Cuadros;Keiko Fujimori Higuchi;Alejandro Toledo Manrique;José Ñique de la Puente;Pedro Pablo Kuczynski;Humberto Pinazo Bella;Rafael Belaúnde Aubry;Oscar Luis Castañeda Lossio</t>
         </is>
       </c>
       <c r="Q112" t="inlineStr">
@@ -26667,7 +26667,7 @@
       </c>
       <c r="P128" t="inlineStr">
         <is>
-          <t>Lino Oviedo;Blanca Odelard;Fernando Lugo;Pedro Fadul</t>
+          <t>Lino Oviedo;Blanca Ovelar;Fernando Lugo;Pedro Fadul</t>
         </is>
       </c>
       <c r="Q128" t="inlineStr">
@@ -34928,7 +34928,7 @@
       </c>
       <c r="P173" t="inlineStr">
         <is>
-          <t>Ricardo Martinelli;Balbina Herrara</t>
+          <t>Ricardo Martinelli;Balbina Herrera</t>
         </is>
       </c>
       <c r="Q173" t="inlineStr">
@@ -59505,7 +59505,7 @@
       </c>
       <c r="N301" t="inlineStr">
         <is>
-          <t>Isabella Mafla;David Ballesteros Ferreira;Juan David Ortiz Luna;Juan Sebastián Lamprea;Luis Ernesto Chia Estupiñan;Nicolás León;Juan Esteban Castañeda;María Alejandra Herrera;Valentina Bohorquez Polo;Juan David Contreras Aragón;Marlon Camilo Barros;Daniel Fabian Otola Martínez;José David Durán Leyva;Gabriela Ortega Navarro;José David Franco</t>
+          <t>Nota de La Nación CR dice: durante el día explicó a la prensa que la "agresión verbal y física" en una anterior visita a la UCR lo obligaron a declinar la invitación para ir al debate. Detalle sobre proceso judicial disponible en: https://www.tse.go.cr/revista/impresa/revista8.pdf</t>
         </is>
       </c>
       <c r="O301">
@@ -59589,7 +59589,7 @@
       </c>
       <c r="AG301" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AH301">
@@ -63091,6 +63091,9 @@
       <c r="E317">
         <v>0</v>
       </c>
+      <c r="F317">
+        <v>1</v>
+      </c>
       <c r="P317" t="inlineStr">
         <is>
           <t>sin datos</t>
@@ -63206,6 +63209,9 @@
       </c>
       <c r="AY317">
         <v>1</v>
+      </c>
+      <c r="AZ317">
+        <v>8</v>
       </c>
     </row>
     <row r="318">
@@ -63223,6 +63229,9 @@
       <c r="E318">
         <v>0</v>
       </c>
+      <c r="F318">
+        <v>1</v>
+      </c>
       <c r="P318" t="inlineStr">
         <is>
           <t>sin datos</t>
@@ -63338,6 +63347,9 @@
       </c>
       <c r="AY318">
         <v>1</v>
+      </c>
+      <c r="AZ318">
+        <v>6</v>
       </c>
     </row>
     <row r="319">
@@ -63355,12 +63367,15 @@
       <c r="E319">
         <v>1</v>
       </c>
+      <c r="F319">
+        <v>1</v>
+      </c>
       <c r="O319">
         <v>2</v>
       </c>
       <c r="P319" t="inlineStr">
         <is>
-          <t>Arias Sánchez;Calderón Fournier</t>
+          <t>Oscar Arias Sanchez;Rafael Calderón Fournier</t>
         </is>
       </c>
       <c r="Q319" t="inlineStr">
@@ -63479,6 +63494,12 @@
       </c>
       <c r="AY319">
         <v>1</v>
+      </c>
+      <c r="AZ319">
+        <v>6</v>
+      </c>
+      <c r="BA319">
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="320">
@@ -63496,6 +63517,9 @@
       <c r="E320">
         <v>0</v>
       </c>
+      <c r="F320">
+        <v>1</v>
+      </c>
       <c r="P320" t="inlineStr">
         <is>
           <t>sin datos</t>
@@ -63611,6 +63635,9 @@
       </c>
       <c r="AY320">
         <v>1</v>
+      </c>
+      <c r="AZ320">
+        <v>8</v>
       </c>
     </row>
     <row r="321">
@@ -63628,6 +63655,9 @@
       <c r="E321">
         <v>0</v>
       </c>
+      <c r="F321">
+        <v>1</v>
+      </c>
       <c r="P321" t="inlineStr">
         <is>
           <t>sin datos</t>
@@ -63743,6 +63773,9 @@
       </c>
       <c r="AY321">
         <v>1</v>
+      </c>
+      <c r="AZ321">
+        <v>7</v>
       </c>
     </row>
     <row r="322">
@@ -64148,6 +64181,11 @@
           <t>Teletica Canal 7</t>
         </is>
       </c>
+      <c r="J324" t="inlineStr">
+        <is>
+          <t>GRAN DEBATE NACIONAL 2002</t>
+        </is>
+      </c>
       <c r="L324" t="inlineStr">
         <is>
           <t>estudio de Canal 7</t>
@@ -64159,11 +64197,11 @@
         </is>
       </c>
       <c r="O324">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="P324" t="inlineStr">
         <is>
-          <t>Nota de La Nación CR dice: durante el día explicó a la prensa que la "agresión verbal y física" en una anterior visita a la UCR lo obligaron a declinar la invitación para ir al debate. REVISAR: ABEL PACHECO ERA PRESIDENTE, NO CANDIDATO</t>
+          <t>el primero: Otto Guevara;Abel Pacheco de la Espriella;Otton Solis;Rolando Araya;el segundo:Pablo Galo Angulo Casasola;José Hine García;Justo Orozco Álvarez;Jorge Walter Coto Molina;Marvin Calvo Montoya;el tercero: Walter Munoz;Daniel Reynolds Vargas;Vladimir de la Cruz de Lemos;Rolando Angulo Zeledón</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -64239,7 +64277,7 @@
         <v>0</v>
       </c>
       <c r="AJ324">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AK324" t="inlineStr">
         <is>
@@ -64318,7 +64356,7 @@
         <v>12</v>
       </c>
       <c r="BA324">
-        <v>0.08333333333333333</v>
+        <v>1.083333333333333</v>
       </c>
     </row>
     <row r="325">
@@ -64994,7 +65032,7 @@
       </c>
       <c r="R328" t="inlineStr">
         <is>
-          <t>cuatro tribunas academicas</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="U328" t="inlineStr">

</xml_diff>

<commit_message>
datos y script datos
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_final1v2023.xlsx
+++ b/tesis_doctorado/datav2023/base_final1v2023.xlsx
@@ -10387,7 +10387,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>TV Gazeta;O Estado de S.Paulo;UOL;Jovem Pan</t>
+          <t>TV Gazeta;O Estado de São Paulo;UOL;Jovem Pan</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -11470,11 +11470,6 @@
           <t>#DebateNaBand</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="L54" t="inlineStr">
         <is>
           <t>estúdio da Band São Paulo</t>
@@ -11689,11 +11684,6 @@
           <t>SBT;CNN Brasil;O Estado de São Paulo;Veja;Terra;NovaBrasil FM</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="L55" t="inlineStr">
         <is>
           <t>nos estúdios do SBT em São Paulo (Osasco)</t>
@@ -12117,11 +12107,6 @@
           <t>Rede Bandeirantes;TV Cultura;FSP;UOL</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="L57" t="inlineStr">
         <is>
           <t>estúdio da Band São Paulo</t>
@@ -12708,7 +12693,7 @@
         <v>1993</v>
       </c>
       <c r="D60" s="2">
-        <v>34275</v>
+        <v>34247</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -12723,17 +12708,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>ANATEL</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>sede del antiguo Congreso Nacional</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>participación de un panel de periodistas representantes de cada canal, un moderador/presentador y público en el estudio</t>
+          <t>Megavision</t>
         </is>
       </c>
       <c r="O60">
@@ -12741,62 +12716,12 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Eduardo Frei Ruiz-Tagle;Arturo Alessandri Besa</t>
+          <t>Manfred Max-Neef;José Piñera</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
           <t>sin ausencias conocidas</t>
-        </is>
-      </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>periodistas;presentes</t>
-        </is>
-      </c>
-      <c r="V60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="X60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="Z60" t="inlineStr">
-        <is>
-          <t>puntuales</t>
-        </is>
-      </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AB60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AC60" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="AD60" t="inlineStr">
-        <is>
-          <t>0.0</t>
         </is>
       </c>
       <c r="AE60">
@@ -12807,84 +12732,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AH60">
-        <v>1</v>
-      </c>
       <c r="AI60">
         <v>0</v>
       </c>
       <c r="AJ60">
         <v>2</v>
-      </c>
-      <c r="AK60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AL60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AM60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AN60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AO60" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AP60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AR60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AS60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AT60" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AU60" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AV60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AW60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AX60" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
       </c>
       <c r="AY60">
         <v>1</v>
@@ -12906,10 +12758,10 @@
         </is>
       </c>
       <c r="C61">
-        <v>2000</v>
+        <v>1993</v>
       </c>
       <c r="D61" s="2">
-        <v>36466</v>
+        <v>34299</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -12924,22 +12776,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>ANATEL</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>hotel de santiago</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>Bernardo Donoso</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>Carolina Jiménez;Felipe Vidal;Juan Manuel Astorga;Claudia Araneda;Mauricio Hoffman;Susana Orno</t>
+          <t>Megavision</t>
         </is>
       </c>
       <c r="O61">
@@ -12947,65 +12784,12 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Joaquín Lavín Infante;Ricardo Lagos Escobar</t>
+          <t>Eugenio Pizzarro;Christian Reitze</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
           <t>sin ausencias conocidas</t>
-        </is>
-      </c>
-      <c r="S61">
-        <v>90</v>
-      </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>periodistas;moderador</t>
-        </is>
-      </c>
-      <c r="V61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="X61" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="Z61" t="inlineStr">
-        <is>
-          <t>bloques;puntuales</t>
-        </is>
-      </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AB61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AC61" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="AD61" t="inlineStr">
-        <is>
-          <t>0.0</t>
         </is>
       </c>
       <c r="AE61">
@@ -13016,98 +12800,20 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AG61" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AH61">
-        <v>1</v>
-      </c>
       <c r="AI61">
         <v>0</v>
       </c>
       <c r="AJ61">
         <v>2</v>
       </c>
-      <c r="AK61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AL61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AM61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AN61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AO61" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AP61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AQ61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AR61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AS61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AT61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AU61" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="AV61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AW61" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AX61" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="AY61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ61">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BA61">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="62">
@@ -13120,10 +12826,10 @@
         </is>
       </c>
       <c r="C62">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="D62" s="2">
-        <v>38621</v>
+        <v>34275</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -13136,47 +12842,27 @@
           <t>FALSE</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>0.458333333333333</t>
-        </is>
-      </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Universidad de Chile</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>"Debate un futuro para la educación chilena"</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>TRUE</t>
+          <t>Chilevisión;TVN;La Red;Megavision;UCTV</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>en el Salón de Honor de la Casa Central</t>
+          <t>sede del antiguo Congreso Nacional</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>Luis Riveros</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>María Teresa Ruiz;Juan Asenjo;Francisco Orrego;Héctor Olav</t>
+          <t>participación de un panel de periodistas representantes de cada canal, un moderador/presentador y público en el estudio</t>
         </is>
       </c>
       <c r="O62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastian Piñera</t>
+          <t>Eduardo Frei Ruiz-Tagle;Arturo Alessandri Besa</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
@@ -13186,17 +12872,17 @@
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>expertos</t>
+          <t>periodistas;presentes</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="W62" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="X62" t="inlineStr">
@@ -13206,12 +12892,12 @@
       </c>
       <c r="Y62" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>monotema</t>
+          <t>puntuales</t>
         </is>
       </c>
       <c r="AA62" t="inlineStr">
@@ -13226,12 +12912,12 @@
       </c>
       <c r="AC62" t="inlineStr">
         <is>
-          <t>Academia</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AD62" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AE62">
@@ -13239,12 +12925,7 @@
       </c>
       <c r="AF62" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AG62" t="inlineStr">
-        <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AH62">
@@ -13254,7 +12935,7 @@
         <v>0</v>
       </c>
       <c r="AJ62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK62" t="inlineStr">
         <is>
@@ -13278,7 +12959,7 @@
       </c>
       <c r="AO62" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AP62" t="inlineStr">
@@ -13288,7 +12969,7 @@
       </c>
       <c r="AQ62" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AR62" t="inlineStr">
@@ -13303,12 +12984,12 @@
       </c>
       <c r="AT62" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AU62" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV62" t="inlineStr">
@@ -13318,7 +12999,7 @@
       </c>
       <c r="AW62" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AX62" t="inlineStr">
@@ -13327,13 +13008,13 @@
         </is>
       </c>
       <c r="AY62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ62">
         <v>4</v>
       </c>
       <c r="BA62">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="63">
@@ -13346,10 +13027,10 @@
         </is>
       </c>
       <c r="C63">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="D63" s="2">
-        <v>38644</v>
+        <v>36466</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -13362,37 +13043,32 @@
           <t>FALSE</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>0.916666666666667</t>
-        </is>
-      </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Canal 13 Pontificia Universidad Católica de Chile;CNN en Español</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>"Foro Presidencial: Chile 2005"</t>
+          <t>ANATEL</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Espacio Riesco, comuna de Huechuraba.</t>
+          <t>hotel de santiago</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>Constanza Santa María;Glenda Umaña</t>
+          <t>Bernardo Donoso</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>Carolina Jiménez;Felipe Vidal;Juan Manuel Astorga;Claudia Araneda;Mauricio Hoffman;Susana Orno</t>
         </is>
       </c>
       <c r="O63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Sebastian Piñera;Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante</t>
+          <t>Joaquín Lavín Infante;Ricardo Lagos Escobar</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
@@ -13401,11 +13077,11 @@
         </is>
       </c>
       <c r="S63">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>periodistas</t>
+          <t>periodistas;moderador</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
@@ -13415,12 +13091,12 @@
       </c>
       <c r="W63" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="X63" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y63" t="inlineStr">
@@ -13430,12 +13106,12 @@
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>puntuales</t>
+          <t>bloques;puntuales</t>
         </is>
       </c>
       <c r="AA63" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AB63" t="inlineStr">
@@ -13458,17 +13134,22 @@
       </c>
       <c r="AF63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
       <c r="AH63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI63">
         <v>0</v>
       </c>
       <c r="AJ63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK63" t="inlineStr">
         <is>
@@ -13537,17 +13218,17 @@
       </c>
       <c r="AX63" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AY63">
         <v>2</v>
       </c>
       <c r="AZ63">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="BA63">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="64">
@@ -13563,7 +13244,7 @@
         <v>2006</v>
       </c>
       <c r="D64" s="2">
-        <v>38672</v>
+        <v>38621</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -13576,24 +13257,39 @@
           <t>FALSE</t>
         </is>
       </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>0.458333333333333</t>
+        </is>
+      </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>ANATEL</t>
+          <t>Universidad de Chile</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>"Debate presidencial 2005"</t>
+          <t>"Debate un futuro para la educación chilena"</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>centro de eventos CasaPiedra, ubicado en la comuna de Vitacura</t>
+          <t>en el Salón de Honor de la Casa Central</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>Mauricio Hofmann;Iván Núñez;Libardo Buitrago;Mauricio Bustamante</t>
+          <t>Luis Riveros</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>María Teresa Ruiz;Juan Asenjo;Francisco Orrego;Héctor Olav</t>
         </is>
       </c>
       <c r="O64">
@@ -13601,7 +13297,7 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Sebastian Piñera;Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante</t>
+          <t>Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastian Piñera</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
@@ -13611,12 +13307,12 @@
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>moderadores</t>
+          <t>expertos</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="W64" t="inlineStr">
@@ -13626,37 +13322,37 @@
       </c>
       <c r="X64" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Y64" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>puntuales</t>
+          <t>monotema</t>
         </is>
       </c>
       <c r="AA64" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AB64" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AC64" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>Academia</t>
         </is>
       </c>
       <c r="AD64" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AE64">
@@ -13667,8 +13363,13 @@
           <t>1</t>
         </is>
       </c>
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="AH64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AI64">
         <v>0</v>
@@ -13693,7 +13394,7 @@
       </c>
       <c r="AN64" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AO64" t="inlineStr">
@@ -13708,7 +13409,7 @@
       </c>
       <c r="AQ64" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AR64" t="inlineStr">
@@ -13728,7 +13429,7 @@
       </c>
       <c r="AU64" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AV64" t="inlineStr">
@@ -13738,7 +13439,7 @@
       </c>
       <c r="AW64" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AX64" t="inlineStr">
@@ -13769,13 +13470,13 @@
         <v>2006</v>
       </c>
       <c r="D65" s="2">
-        <v>38721</v>
+        <v>38644</v>
       </c>
       <c r="E65">
         <v>1</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -13789,25 +13490,30 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>ANATEL</t>
+          <t>Canal 13 Pontificia Universidad Católica de Chile;CNN en Español</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>"Foro Presidencial: Chile 2005"</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Espacio Riesco a las 22 (UTC-3).</t>
+          <t>Espacio Riesco, comuna de Huechuraba.</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>Amaro Gómez-Pablos;Libardo Buitrago;Alejandro Guillier;Constanza Santa María</t>
+          <t>Constanza Santa María;Glenda Umaña</t>
         </is>
       </c>
       <c r="O65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Sebastian Piñera;Michelle Bachelet</t>
+          <t>Sebastian Piñera;Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
@@ -13815,9 +13521,12 @@
           <t>sin ausencias conocidas</t>
         </is>
       </c>
+      <c r="S65">
+        <v>60</v>
+      </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>moderadores</t>
+          <t>periodistas</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
@@ -13870,17 +13579,17 @@
       </c>
       <c r="AF65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AH65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI65">
         <v>0</v>
       </c>
       <c r="AJ65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK65" t="inlineStr">
         <is>
@@ -13899,12 +13608,12 @@
       </c>
       <c r="AN65" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AO65" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AP65" t="inlineStr">
@@ -13956,7 +13665,7 @@
         <v>2</v>
       </c>
       <c r="AZ65">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BA65">
         <v>1</v>
@@ -13975,7 +13684,7 @@
         <v>2006</v>
       </c>
       <c r="D66" s="2">
-        <v>38685</v>
+        <v>38672</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -13983,64 +13692,92 @@
       <c r="F66">
         <v>1</v>
       </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>ENADE / ICARE</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>DUDA</t>
-        </is>
+          <t>ANATEL</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>"Debate presidencial 2005"</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>centro de eventos CasaPiedra, ubicado en la comuna de Vitacura</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>Mauricio Hofmann;Iván Núñez;Libardo Buitrago;Mauricio Bustamante</t>
+        </is>
+      </c>
+      <c r="O66">
+        <v>4</v>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>sin datos</t>
+          <t>Sebastian Piñera;Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>sin datos</t>
+          <t>sin ausencias conocidas</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>moderadores</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="X66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Y66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>puntuales</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AB66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="AC66" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AE66">
@@ -14051,74 +13788,83 @@
           <t>1</t>
         </is>
       </c>
+      <c r="AH66">
+        <v>4</v>
+      </c>
+      <c r="AI66">
+        <v>0</v>
+      </c>
+      <c r="AJ66">
+        <v>4</v>
+      </c>
       <c r="AK66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AL66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AM66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AN66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AO66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AP66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AQ66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AR66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AS66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AT66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AU66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AW66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AX66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AY66">
@@ -14126,6 +13872,9 @@
       </c>
       <c r="AZ66">
         <v>4</v>
+      </c>
+      <c r="BA66">
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -14141,35 +13890,45 @@
         <v>2006</v>
       </c>
       <c r="D67" s="2">
-        <v>38650</v>
+        <v>38721</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0.916666666666667</t>
+        </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>ComunidadMujer</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>DUDA</t>
+          <t>ANATEL</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>edificio "Diego Portales"</t>
+          <t>Espacio Riesco a las 22 (UTC-3).</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>Amaro Gómez-Pablos;Libardo Buitrago;Alejandro Guillier;Constanza Santa María</t>
         </is>
       </c>
       <c r="O67">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastian Piñera</t>
+          <t>Sebastian Piñera;Michelle Bachelet</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
@@ -14179,42 +13938,52 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>moderadores</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="W67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="X67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Y67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>monotema</t>
+          <t>puntuales</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AB67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AE67">
@@ -14225,65 +13994,68 @@
           <t>1</t>
         </is>
       </c>
+      <c r="AH67">
+        <v>4</v>
+      </c>
       <c r="AI67">
         <v>0</v>
       </c>
       <c r="AJ67">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AL67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AM67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AN67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AO67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AP67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AQ67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AR67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AS67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AT67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AU67" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV67" t="inlineStr">
@@ -14293,7 +14065,7 @@
       </c>
       <c r="AW67" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AX67" t="inlineStr">
@@ -14305,7 +14077,7 @@
         <v>2</v>
       </c>
       <c r="AZ67">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BA67">
         <v>1</v>
@@ -14321,10 +14093,10 @@
         </is>
       </c>
       <c r="C68">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D68" s="2">
-        <v>40081</v>
+        <v>38685</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -14334,40 +14106,27 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>ComunidadMujer</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>“Voz de Mujer 2010”</t>
+          <t>ENADE / ICARE</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>Monica Perez</t>
-        </is>
-      </c>
-      <c r="O68">
-        <v>4</v>
+          <t>DUDA</t>
+        </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami ;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
+          <t>sin datos</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>sin ausencias conocidas</t>
+          <t>sin datos</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>vrituales</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
@@ -14377,12 +14136,12 @@
       </c>
       <c r="W68" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
@@ -14392,27 +14151,17 @@
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>monotema</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AB68" t="inlineStr">
         <is>
           <t>NA</t>
-        </is>
-      </c>
-      <c r="AC68" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-      <c r="AD68" t="inlineStr">
-        <is>
-          <t>3.0</t>
         </is>
       </c>
       <c r="AE68">
@@ -14423,83 +14172,74 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AH68">
-        <v>1</v>
-      </c>
-      <c r="AI68">
-        <v>0</v>
-      </c>
-      <c r="AJ68">
-        <v>4</v>
-      </c>
       <c r="AK68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AL68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AM68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AN68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AO68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AP68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AQ68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AR68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AS68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AT68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AU68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AV68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AW68" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AX68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AY68">
@@ -14507,9 +14247,6 @@
       </c>
       <c r="AZ68">
         <v>4</v>
-      </c>
-      <c r="BA68">
-        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -14522,10 +14259,10 @@
         </is>
       </c>
       <c r="C69">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D69" s="2">
-        <v>40079</v>
+        <v>38650</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -14533,24 +14270,19 @@
       <c r="F69">
         <v>1</v>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>0.944444444444444</t>
-        </is>
-      </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>TVN</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>"Decisión '09"</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>Alejandro Guillier</t>
+          <t>ComunidadMujer</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>DUDA</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>edificio "Diego Portales"</t>
         </is>
       </c>
       <c r="O69">
@@ -14558,7 +14290,7 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
+          <t>Michelle Bachelet;Tomás Hirsch Goldschmidt;Joaquín Lavín Infante;Sebastian Piñera</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
@@ -14568,52 +14300,42 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>moderadores</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="X69" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Y69" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>puntuales</t>
+          <t>monotema</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AB69" t="inlineStr">
         <is>
           <t>NA</t>
-        </is>
-      </c>
-      <c r="AC69" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="AD69" t="inlineStr">
-        <is>
-          <t>0.0</t>
         </is>
       </c>
       <c r="AE69">
@@ -14624,9 +14346,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AH69">
-        <v>1</v>
-      </c>
       <c r="AI69">
         <v>0</v>
       </c>
@@ -14635,57 +14354,57 @@
       </c>
       <c r="AK69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AL69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AM69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AN69" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AO69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AP69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AQ69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AR69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AS69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AT69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AU69" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AV69" t="inlineStr">
@@ -14695,7 +14414,7 @@
       </c>
       <c r="AW69" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AX69" t="inlineStr">
@@ -14726,7 +14445,7 @@
         <v>2010</v>
       </c>
       <c r="D70" s="2">
-        <v>40095</v>
+        <v>40081</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -14734,29 +14453,24 @@
       <c r="F70">
         <v>1</v>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>0.354166666666667</t>
-        </is>
-      </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>ARCHI;Universidad Mayor</t>
+          <t>ComunidadMujer</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>“Voz de Mujer 2010”</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>DUDA</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Campus de la Universidad</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>Alejandro de la Carrera;Verónica Franco;Cony Stipicic;Beatriz Sánche</t>
+          <t>Monica Perez</t>
         </is>
       </c>
       <c r="O70">
@@ -14772,17 +14486,14 @@
           <t>sin ausencias conocidas</t>
         </is>
       </c>
-      <c r="S70">
-        <v>80</v>
-      </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>moderadores</t>
+          <t>vrituales</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
@@ -14797,12 +14508,12 @@
       </c>
       <c r="Y70" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>puntuales</t>
+          <t>monotema</t>
         </is>
       </c>
       <c r="AA70" t="inlineStr">
@@ -14812,17 +14523,17 @@
       </c>
       <c r="AB70" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>Mujeres</t>
         </is>
       </c>
       <c r="AD70" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AE70">
@@ -14830,11 +14541,11 @@
       </c>
       <c r="AF70" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AH70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AI70">
         <v>0</v>
@@ -14859,7 +14570,7 @@
       </c>
       <c r="AN70" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AO70" t="inlineStr">
@@ -14894,7 +14605,7 @@
       </c>
       <c r="AU70" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AV70" t="inlineStr">
@@ -14904,7 +14615,7 @@
       </c>
       <c r="AW70" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AX70" t="inlineStr">
@@ -14935,7 +14646,7 @@
         <v>2010</v>
       </c>
       <c r="D71" s="2">
-        <v>40123</v>
+        <v>40079</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -14945,32 +14656,22 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>0.375</t>
+          <t>0.944444444444444</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>ANP Asociación Nacional de la Prensa</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>por primera vez en regiones. ciudad de Talca. En Hotel Casino</t>
+          <t>TVN</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>"Decisión '09"</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>Guillermo Turner</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>Francisco Puga;Antonio Faundes;Mauricio Rivas;Alejandro Toro</t>
+          <t>Alejandro Guillier</t>
         </is>
       </c>
       <c r="O71">
@@ -14978,7 +14679,7 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami ;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
+          <t>Jorge Arrate Mac Niven;Marco Enríquez-Ominami;Sebastian Piñera;Eduardo Frei Ruiz-Tagle</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
@@ -14986,27 +14687,24 @@
           <t>sin ausencias conocidas</t>
         </is>
       </c>
-      <c r="S71">
-        <v>120</v>
-      </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>periodistas</t>
+          <t>moderadores</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="W71" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="X71" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y71" t="inlineStr">
@@ -15016,17 +14714,27 @@
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>monotema</t>
+          <t>puntuales</t>
         </is>
       </c>
       <c r="AA71" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AB71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="AD71" t="inlineStr">
+        <is>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AE71">
@@ -15037,11 +14745,6 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AG71" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="AH71">
         <v>1</v>
       </c>
@@ -15068,12 +14771,12 @@
       </c>
       <c r="AN71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AO71" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AP71" t="inlineStr">
@@ -15103,7 +14806,7 @@
       </c>
       <c r="AU71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV71" t="inlineStr">
@@ -15113,7 +14816,7 @@
       </c>
       <c r="AW71" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AX71" t="inlineStr">
@@ -15144,7 +14847,7 @@
         <v>2010</v>
       </c>
       <c r="D72" s="2">
-        <v>40126</v>
+        <v>40095</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -15154,27 +14857,27 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>0.916666666666667</t>
+          <t>0.354166666666667</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>Canal 13 Pontificia Universidad Católica de Chile</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>"Chile Debate"</t>
+          <t>ARCHI;Universidad Mayor</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>DUDA</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>estudio de Canal 13</t>
+          <t>Campus de la Universidad</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>Daniel Matamala;Constanza Santa María</t>
+          <t>Alejandro de la Carrera;Verónica Franco;Cony Stipicic;Beatriz Sánche</t>
         </is>
       </c>
       <c r="O72">
@@ -15191,26 +14894,26 @@
         </is>
       </c>
       <c r="S72">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>moderadores;presentes;duelo</t>
+          <t>moderadores</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="X72" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Y72" t="inlineStr">
@@ -15220,12 +14923,12 @@
       </c>
       <c r="Z72" t="inlineStr">
         <is>
-          <t>puntuales;libre</t>
+          <t>puntuales</t>
         </is>
       </c>
       <c r="AA72" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AB72" t="inlineStr">
@@ -15248,11 +14951,11 @@
       </c>
       <c r="AF72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AH72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AI72">
         <v>0</v>
@@ -15272,7 +14975,7 @@
       </c>
       <c r="AM72" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AN72" t="inlineStr">
@@ -15307,7 +15010,7 @@
       </c>
       <c r="AT72" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AU72" t="inlineStr">
@@ -15317,7 +15020,7 @@
       </c>
       <c r="AV72" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="AW72" t="inlineStr">
@@ -18796,11 +18499,6 @@
           <t>#DebateCHVCNN</t>
         </is>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="M90" t="inlineStr">
         <is>
           <t>Mónica Rincón;Daniel Matamala</t>
@@ -19575,11 +19273,6 @@
           <t>Futuro del agua #DebateAguaXLARED</t>
         </is>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="M94" t="inlineStr">
         <is>
           <t>Julia Vial</t>
@@ -19799,11 +19492,6 @@
           <t>Debate Universidad de Chile 2021  #DebateUchile</t>
         </is>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="M95" t="inlineStr">
         <is>
           <t>Mariela Ravanal</t>
@@ -22059,7 +21747,7 @@
       </c>
       <c r="AU105" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV105" t="inlineStr">
@@ -22278,7 +21966,7 @@
       </c>
       <c r="AU106" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV106" t="inlineStr">
@@ -28039,7 +27727,7 @@
       </c>
       <c r="AU134" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV134" t="inlineStr">
@@ -31136,7 +30824,7 @@
       </c>
       <c r="AU150" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV150" t="inlineStr">
@@ -46694,7 +46382,7 @@
       </c>
       <c r="AU236" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV236" t="inlineStr">
@@ -46913,7 +46601,7 @@
       </c>
       <c r="AU237" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV237" t="inlineStr">
@@ -47121,7 +46809,7 @@
       </c>
       <c r="AU238" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV238" t="inlineStr">
@@ -47332,7 +47020,7 @@
       </c>
       <c r="AU239" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV239" t="inlineStr">
@@ -47486,7 +47174,7 @@
       </c>
       <c r="AU240" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV240" t="inlineStr">
@@ -47705,7 +47393,7 @@
       </c>
       <c r="AU241" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV241" t="inlineStr">
@@ -47924,7 +47612,7 @@
       </c>
       <c r="AU242" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV242" t="inlineStr">
@@ -48128,7 +47816,7 @@
       </c>
       <c r="AU243" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV243" t="inlineStr">
@@ -48341,7 +48029,7 @@
       </c>
       <c r="AU244" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="AV244" t="inlineStr">
@@ -50263,7 +49951,7 @@
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>Comisión Nacional de Televisión</t>
+          <t>Comisión Nacional de Televisión;Alianza MMC</t>
         </is>
       </c>
       <c r="J255" t="inlineStr">
@@ -50347,7 +50035,7 @@
       </c>
       <c r="AF255" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AG255" t="inlineStr">
@@ -50472,7 +50160,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>Comisión Nacional de Televisión</t>
+          <t>Comisión Nacional de Televisión;Alianza MMC</t>
         </is>
       </c>
       <c r="J256" t="inlineStr">
@@ -50551,7 +50239,7 @@
       </c>
       <c r="AF256" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AH256">
@@ -74069,11 +73757,6 @@
       <c r="J372" t="inlineStr">
         <is>
           <t>#LaDiscusiónPresidencial</t>
-        </is>
-      </c>
-      <c r="K372" t="inlineStr">
-        <is>
-          <t>TRUE</t>
         </is>
       </c>
       <c r="L372" t="inlineStr">

</xml_diff>